<commit_message>
Updated for issue #1.  Routing parser and VRF parsers were not working correctly.
</commit_message>
<xml_diff>
--- a/GetInventory - Default.xlsx
+++ b/GetInventory - Default.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insightonline-my.sharepoint.com/personal/ruben_gutierrezmartinez_insight_com/Documents/Documents/GitHub/GetInventory/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tony\PycharmProjects\GetInventory_InsightSSG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{3BF8DEBB-66D5-4598-82DF-D5459BDD8E12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3DAEDAF1-643A-4BA0-A2F9-24005E5BF250}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3763158-9B3B-4CCA-8F0E-C2B9F6C63225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="849" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33780" yWindow="2700" windowWidth="28800" windowHeight="15460" tabRatio="849" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="185">
   <si>
     <t>Username</t>
   </si>
@@ -595,6 +595,18 @@
   </si>
   <si>
     <t>Elapsed Time (Seconds)</t>
+  </si>
+  <si>
+    <t>192.168.1.192</t>
+  </si>
+  <si>
+    <t>cisco_ios</t>
+  </si>
+  <si>
+    <t>ssh</t>
+  </si>
+  <si>
+    <t>cisco</t>
   </si>
 </sst>
 </file>
@@ -859,23 +871,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment textRotation="60"/>
       <protection locked="0"/>
@@ -900,9 +903,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -1303,560 +1303,571 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:BA14"/>
+  <dimension ref="A1:BA8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" style="16" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="7" style="16" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" style="16" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" style="16" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="16" customWidth="1"/>
-    <col min="10" max="10" width="25.21875" style="16" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" style="16" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="16" customWidth="1"/>
-    <col min="13" max="13" width="8.77734375" style="16"/>
-    <col min="14" max="14" width="16" style="16" customWidth="1"/>
-    <col min="15" max="15" width="20" style="16" customWidth="1"/>
-    <col min="16" max="16" width="16" style="16" customWidth="1"/>
-    <col min="17" max="17" width="51.21875" style="16" customWidth="1"/>
-    <col min="18" max="34" width="4.21875" style="16" customWidth="1"/>
-    <col min="35" max="45" width="4.44140625" style="16" customWidth="1"/>
-    <col min="46" max="47" width="8.77734375" style="16"/>
-    <col min="48" max="48" width="16.77734375" style="16" customWidth="1"/>
-    <col min="49" max="49" width="74.21875" style="16" customWidth="1"/>
-    <col min="50" max="50" width="54.5546875" style="16" customWidth="1"/>
-    <col min="51" max="51" width="37.21875" style="16" customWidth="1"/>
-    <col min="52" max="52" width="37.77734375" style="16" customWidth="1"/>
-    <col min="53" max="53" width="8.77734375" style="16"/>
-    <col min="54" max="16384" width="8.77734375" style="15"/>
+    <col min="1" max="1" width="20.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.81640625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="7" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="20.54296875" style="9" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="25.1796875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.54296875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="9"/>
+    <col min="14" max="14" width="16" style="9" customWidth="1"/>
+    <col min="15" max="15" width="20" style="9" customWidth="1"/>
+    <col min="16" max="16" width="16" style="9" customWidth="1"/>
+    <col min="17" max="17" width="51.1796875" style="9" customWidth="1"/>
+    <col min="18" max="34" width="4.1796875" style="9" customWidth="1"/>
+    <col min="35" max="45" width="4.453125" style="9" customWidth="1"/>
+    <col min="46" max="47" width="8.81640625" style="9"/>
+    <col min="48" max="48" width="16.81640625" style="9" customWidth="1"/>
+    <col min="49" max="49" width="74.1796875" style="9" customWidth="1"/>
+    <col min="50" max="50" width="54.54296875" style="9" customWidth="1"/>
+    <col min="51" max="51" width="37.1796875" style="9" customWidth="1"/>
+    <col min="52" max="52" width="37.81640625" style="9" customWidth="1"/>
+    <col min="53" max="53" width="8.81640625" style="9"/>
+    <col min="54" max="16384" width="8.81640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:53" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="28" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AG1" s="15"/>
-      <c r="AH1" s="15"/>
-      <c r="AI1" s="15"/>
-      <c r="AJ1" s="15"/>
-      <c r="AK1" s="15"/>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-      <c r="AP1" s="15"/>
-      <c r="AQ1" s="15"/>
-      <c r="AR1" s="15"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="15"/>
-      <c r="AW1" s="15"/>
-      <c r="AX1" s="15"/>
-      <c r="AY1" s="15"/>
-      <c r="AZ1" s="15"/>
-      <c r="BA1" s="15"/>
-    </row>
-    <row r="2" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="K1" s="20"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8"/>
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8"/>
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+    </row>
+    <row r="2" spans="1:53" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="29" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="15"/>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="15"/>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="15"/>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-    </row>
-    <row r="3" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+    </row>
+    <row r="3" spans="1:53" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
-      <c r="AC3" s="15"/>
-      <c r="AD3" s="15"/>
-      <c r="AE3" s="15"/>
-      <c r="AF3" s="15"/>
-      <c r="AG3" s="15"/>
-      <c r="AH3" s="15"/>
-      <c r="AI3" s="15"/>
-      <c r="AJ3" s="15"/>
-      <c r="AK3" s="15"/>
-      <c r="AL3" s="15"/>
-      <c r="AM3" s="15"/>
-      <c r="AN3" s="15"/>
-      <c r="AO3" s="15"/>
-      <c r="AP3" s="15"/>
-      <c r="AQ3" s="15"/>
-      <c r="AR3" s="15"/>
-      <c r="AS3" s="15"/>
-      <c r="AT3" s="15"/>
-      <c r="AU3" s="15"/>
-      <c r="AV3" s="15"/>
-      <c r="AW3" s="15"/>
-      <c r="AX3" s="15"/>
-      <c r="AY3" s="15"/>
-      <c r="AZ3" s="15"/>
-      <c r="BA3" s="15"/>
-    </row>
-    <row r="4" spans="1:53" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="8"/>
+    </row>
+    <row r="4" spans="1:53" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
-      <c r="AB4" s="15"/>
-      <c r="AC4" s="15"/>
-      <c r="AD4" s="15"/>
-      <c r="AE4" s="15"/>
-      <c r="AF4" s="15"/>
-      <c r="AG4" s="15"/>
-      <c r="AH4" s="15"/>
-      <c r="AI4" s="15"/>
-      <c r="AJ4" s="15"/>
-      <c r="AK4" s="15"/>
-      <c r="AL4" s="15"/>
-      <c r="AM4" s="15"/>
-      <c r="AN4" s="15"/>
-      <c r="AO4" s="15"/>
-      <c r="AP4" s="15"/>
-      <c r="AQ4" s="15"/>
-      <c r="AR4" s="15"/>
-      <c r="AS4" s="15"/>
-      <c r="AT4" s="15"/>
-      <c r="AU4" s="15"/>
-      <c r="AV4" s="15"/>
-      <c r="AW4" s="15"/>
-      <c r="AX4" s="15"/>
-      <c r="AY4" s="15"/>
-      <c r="AZ4" s="15"/>
-      <c r="BA4" s="15"/>
-    </row>
-    <row r="5" spans="1:53" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="8"/>
+      <c r="AQ4" s="8"/>
+      <c r="AR4" s="8"/>
+      <c r="AS4" s="8"/>
+      <c r="AT4" s="8"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="8"/>
+      <c r="BA4" s="8"/>
+    </row>
+    <row r="5" spans="1:53" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="18" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="15"/>
-      <c r="AC5" s="15"/>
-      <c r="AD5" s="15"/>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="15"/>
-      <c r="AJ5" s="15"/>
-      <c r="AK5" s="15"/>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15"/>
-      <c r="AO5" s="15"/>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="15"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="15"/>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="15"/>
-      <c r="AV5" s="15"/>
-      <c r="AW5" s="15"/>
-      <c r="AX5" s="15"/>
-      <c r="AY5" s="15"/>
-      <c r="AZ5" s="15"/>
-      <c r="BA5" s="15"/>
-    </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
-      <c r="AB6" s="15"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="15"/>
-      <c r="AE6" s="15"/>
-      <c r="AF6" s="15"/>
-      <c r="AG6" s="15"/>
-      <c r="AH6" s="15"/>
-      <c r="AI6" s="15"/>
-      <c r="AJ6" s="15"/>
-      <c r="AK6" s="15"/>
-      <c r="AL6" s="15"/>
-      <c r="AM6" s="15"/>
-      <c r="AN6" s="15"/>
-      <c r="AO6" s="15"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
-      <c r="AW6" s="15"/>
-      <c r="AX6" s="15"/>
-      <c r="AY6" s="15"/>
-      <c r="AZ6" s="15"/>
-      <c r="BA6" s="15"/>
-    </row>
-    <row r="7" spans="1:53" ht="109.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
+      <c r="AN5" s="8"/>
+      <c r="AO5" s="8"/>
+      <c r="AP5" s="8"/>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="8"/>
+      <c r="AS5" s="8"/>
+      <c r="AT5" s="8"/>
+      <c r="AU5" s="8"/>
+      <c r="AV5" s="8"/>
+      <c r="AW5" s="8"/>
+      <c r="AX5" s="8"/>
+      <c r="AY5" s="8"/>
+      <c r="AZ5" s="8"/>
+      <c r="BA5" s="8"/>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.35">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="8"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="8"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="AZ6" s="8"/>
+      <c r="BA6" s="8"/>
+    </row>
+    <row r="7" spans="1:53" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="T7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="V7" s="13" t="s">
+      <c r="V7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="W7" s="13" t="s">
+      <c r="W7" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="X7" s="13" t="s">
+      <c r="X7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="Y7" s="13" t="s">
+      <c r="Y7" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="Z7" s="13" t="s">
+      <c r="Z7" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="AA7" s="13" t="s">
+      <c r="AA7" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="AB7" s="13" t="s">
+      <c r="AB7" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AC7" s="13" t="s">
+      <c r="AC7" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="AD7" s="13" t="s">
+      <c r="AD7" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="AE7" s="13" t="s">
+      <c r="AE7" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="AF7" s="13" t="s">
+      <c r="AF7" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="AG7" s="13" t="s">
+      <c r="AG7" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="AH7" s="13" t="s">
+      <c r="AH7" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="AI7" s="13" t="s">
+      <c r="AI7" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="AJ7" s="13" t="s">
+      <c r="AJ7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AK7" s="13" t="s">
+      <c r="AK7" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="AL7" s="13" t="s">
+      <c r="AL7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AM7" s="13" t="s">
+      <c r="AM7" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="AN7" s="13" t="s">
+      <c r="AN7" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AO7" s="13" t="s">
+      <c r="AO7" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="AP7" s="13" t="s">
+      <c r="AP7" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AQ7" s="13" t="s">
+      <c r="AQ7" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="AR7" s="14" t="s">
+      <c r="AR7" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="AS7" s="14" t="s">
+      <c r="AS7" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="AT7" s="14" t="s">
+      <c r="AT7" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="AU7" s="14" t="s">
+      <c r="AU7" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AV7" s="10" t="s">
+      <c r="AV7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="AW7" s="10" t="s">
+      <c r="AW7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AX7" s="10" t="s">
+      <c r="AX7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AY7" s="10" t="s">
+      <c r="AY7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AZ7" s="10" t="s">
+      <c r="AZ7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BA7" s="10" t="s">
+      <c r="BA7" s="3" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
-    </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>184</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -1900,153 +1911,153 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.21875" customWidth="1"/>
+    <col min="1" max="1" width="32.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>133</v>
       </c>
     </row>
@@ -2062,169 +2073,164 @@
   </sheetPr>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" style="3" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" style="18" customWidth="1"/>
-    <col min="4" max="5" width="9.21875" style="18"/>
-    <col min="6" max="6" width="53.77734375" style="18" customWidth="1"/>
-    <col min="7" max="16384" width="9.21875" style="18"/>
+    <col min="1" max="1" width="19.81640625" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="30.81640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" style="10" customWidth="1"/>
+    <col min="4" max="5" width="9.1796875" style="10"/>
+    <col min="6" max="6" width="53.81640625" style="10" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A1" s="9"/>
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:7" ht="31" x14ac:dyDescent="0.7">
+      <c r="B1" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="35" t="s">
+    <row r="2" spans="1:7" ht="58.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="C2" s="35"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="C2" s="27"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>170</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>136</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="34"/>
-      <c r="G5" s="22"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>137</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>150</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="34"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>138</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>149</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="34"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="F7" s="26"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>139</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="34"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="F8" s="26"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>140</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="34"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="F9" s="26"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>141</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>148</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="34"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="26"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>142</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>143</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>144</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>145</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" t="s">
         <v>146</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>147</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>178</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" t="s">
         <v>179</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="2">
         <v>10</v>
       </c>
     </row>
@@ -2260,14 +2266,14 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="135.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+    <col min="3" max="3" width="135.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2293,30 +2299,29 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="66.77734375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.21875" style="3"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="4" max="4" width="66.81640625" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>134</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2335,36 +2340,36 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" customWidth="1"/>
-    <col min="4" max="4" width="44.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.77734375" customWidth="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" customWidth="1"/>
+    <col min="4" max="4" width="44.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+    <col min="8" max="14" width="16.1796875" customWidth="1"/>
+    <col min="15" max="15" width="15.1796875" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="9.21875" style="1"/>
-    <col min="18" max="18" width="15.77734375" customWidth="1"/>
-    <col min="19" max="19" width="13.44140625" customWidth="1"/>
+    <col min="17" max="17" width="9.1796875" style="1"/>
+    <col min="18" max="18" width="15.81640625" customWidth="1"/>
+    <col min="19" max="19" width="13.453125" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
-    <col min="22" max="22" width="13.21875" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.1796875" customWidth="1"/>
+    <col min="23" max="23" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2476,19 +2481,19 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
-    <col min="6" max="8" width="17.21875" customWidth="1"/>
-    <col min="9" max="10" width="17.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="1" customWidth="1"/>
+    <col min="6" max="8" width="17.1796875" customWidth="1"/>
+    <col min="9" max="10" width="17.1796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2540,48 +2545,47 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.21875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="20" style="9" customWidth="1"/>
-    <col min="6" max="16384" width="9.21875" style="9"/>
+    <col min="1" max="1" width="25.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.1796875" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" t="s">
         <v>159</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" t="s">
         <v>160</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" t="s">
         <v>162</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" t="s">
         <v>163</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" t="s">
         <v>165</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" t="s">
         <v>166</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" t="s">
         <v>167</v>
       </c>
     </row>
@@ -2600,20 +2604,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.21875" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="3" width="24.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" customWidth="1"/>
-    <col min="8" max="8" width="138.5546875" customWidth="1"/>
-    <col min="9" max="9" width="100.44140625" customWidth="1"/>
+    <col min="7" max="7" width="20.81640625" customWidth="1"/>
+    <col min="8" max="8" width="138.54296875" customWidth="1"/>
+    <col min="9" max="9" width="100.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2657,18 +2661,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2706,14 +2710,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" customWidth="1"/>
-    <col min="5" max="5" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="27.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2747,49 +2751,47 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.21875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="24.21875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="46.77734375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="17" style="7" customWidth="1"/>
-    <col min="8" max="8" width="138.5546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="19" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="9.21875" style="7"/>
+    <col min="1" max="2" width="24.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.81640625" customWidth="1"/>
+    <col min="4" max="4" width="46.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" customWidth="1"/>
+    <col min="6" max="6" width="30.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
+    <col min="8" max="8" width="138.54296875" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" t="s">
         <v>154</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2797,4 +2799,10 @@
   <autoFilter ref="A1:H1" xr:uid="{B7EB6E73-7A47-4B22-A88C-5BA601D79630}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{f956267e-7d50-46d0-9b27-8f911a5b38ff}" enabled="1" method="Standard" siteId="{6c637512-c417-4e78-9d62-b61258e4b619}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>